<commit_message>
update basics of programming
</commit_message>
<xml_diff>
--- a/code/02_basics_of_programming/GDP_by_country.xlsx
+++ b/code/02_basics_of_programming/GDP_by_country.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/5610710/Documents/data_school/SummerSchool24/Summer-School-2024/code/02_basics_of_programming/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{CD055BDE-B2ED-CA43-8606-3D8D181B62E5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{62FB26FA-F21B-2D40-98BC-ECD90B73FFC0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1560" yWindow="-18240" windowWidth="27640" windowHeight="16660" xr2:uid="{7297F4C7-2824-1340-92D3-1473E0ECEC47}"/>
   </bookViews>
@@ -36,14 +36,11 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="313" uniqueCount="198">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="306" uniqueCount="194">
   <si>
     <t>Country</t>
   </si>
   <si>
-    <t>Info</t>
-  </si>
-  <si>
     <t>Afghanistan</t>
   </si>
   <si>
@@ -80,9 +77,6 @@
     <t>Bahamas</t>
   </si>
   <si>
-    <t xml:space="preserve"> a</t>
-  </si>
-  <si>
     <t>Bahrain</t>
   </si>
   <si>
@@ -524,9 +518,6 @@
     <t>South Sudan</t>
   </si>
   <si>
-    <t xml:space="preserve"> b</t>
-  </si>
-  <si>
     <t>Spain</t>
   </si>
   <si>
@@ -603,9 +594,6 @@
   </si>
   <si>
     <t>Venezuela (Bolivarian Republic of)</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> c</t>
   </si>
   <si>
     <t>Viet Nam</t>
@@ -1032,10 +1020,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{326A2443-8483-5147-9601-40878C23E5F1}">
-  <dimension ref="A1:O210"/>
+  <dimension ref="A1:N210"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G10" sqref="G10"/>
+      <selection activeCell="Q8" sqref="Q8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1043,10 +1031,9 @@
     <col min="1" max="1" width="12.5" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="12.5" style="5" bestFit="1" customWidth="1"/>
     <col min="3" max="14" width="12.5" style="6" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="12.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:14" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1089,22 +1076,19 @@
       <c r="N1" s="1">
         <v>2018</v>
       </c>
-      <c r="O1" t="s">
+    </row>
+    <row r="2" spans="1:14" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="2" spans="1:15" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
-        <v>2</v>
-      </c>
       <c r="B2" s="1" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E2" s="2">
         <v>28.2</v>
@@ -1137,9 +1121,9 @@
         <v>64.5</v>
       </c>
     </row>
-    <row r="3" spans="1:15" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:14" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B3" s="2">
         <v>14.7</v>
@@ -1181,9 +1165,9 @@
         <v>35.299999999999997</v>
       </c>
     </row>
-    <row r="4" spans="1:15" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:14" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B4" s="2">
         <v>265.3</v>
@@ -1225,9 +1209,9 @@
         <v>586.4</v>
       </c>
     </row>
-    <row r="5" spans="1:15" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:14" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B5" s="2">
         <v>56.4</v>
@@ -1269,9 +1253,9 @@
         <v>176.4</v>
       </c>
     </row>
-    <row r="6" spans="1:15" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:14" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B6" s="2">
         <v>1.1000000000000001</v>
@@ -1313,9 +1297,9 @@
         <v>2.2999999999999998</v>
       </c>
     </row>
-    <row r="7" spans="1:15" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:14" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B7" s="1">
         <v>371</v>
@@ -1357,9 +1341,9 @@
         <v>813.5</v>
       </c>
     </row>
-    <row r="8" spans="1:15" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:14" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B8" s="2">
         <v>13.2</v>
@@ -1401,9 +1385,9 @@
         <v>27.1</v>
       </c>
     </row>
-    <row r="9" spans="1:15" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:14" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B9" s="2">
         <v>489.2</v>
@@ -1445,9 +1429,9 @@
         <v>1135.5999999999999</v>
       </c>
     </row>
-    <row r="10" spans="1:15" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:14" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B10" s="2">
         <v>240.6</v>
@@ -1489,9 +1473,9 @@
         <v>411.2</v>
       </c>
     </row>
-    <row r="11" spans="1:15" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:14" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B11" s="2">
         <v>62.9</v>
@@ -1533,9 +1517,9 @@
         <v>159.19999999999999</v>
       </c>
     </row>
-    <row r="12" spans="1:15" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:14" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B12" s="2">
         <v>7.9</v>
@@ -1576,13 +1560,10 @@
       <c r="N12" s="1">
         <v>11</v>
       </c>
-      <c r="O12" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="13" spans="1:15" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="13" spans="1:14" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="B13" s="2">
         <v>17.399999999999999</v>
@@ -1624,9 +1605,9 @@
         <v>65.900000000000006</v>
       </c>
     </row>
-    <row r="14" spans="1:15" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:14" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="B14" s="2">
         <v>136.80000000000001</v>
@@ -1668,9 +1649,9 @@
         <v>625.9</v>
       </c>
     </row>
-    <row r="15" spans="1:15" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:14" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="B15" s="2">
         <v>3.7</v>
@@ -1711,13 +1692,10 @@
       <c r="N15" s="2">
         <v>4.8</v>
       </c>
-      <c r="O15" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="16" spans="1:15" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="16" spans="1:14" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="B16" s="2">
         <v>85.2</v>
@@ -1761,7 +1739,7 @@
     </row>
     <row r="17" spans="1:14" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="B17" s="2">
         <v>305.5</v>
@@ -1805,7 +1783,7 @@
     </row>
     <row r="18" spans="1:14" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="B18" s="1">
         <v>1</v>
@@ -1849,7 +1827,7 @@
     </row>
     <row r="19" spans="1:14" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="B19" s="2">
         <v>7.3</v>
@@ -1893,7 +1871,7 @@
     </row>
     <row r="20" spans="1:14" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="B20" s="2">
         <v>1.2</v>
@@ -1937,7 +1915,7 @@
     </row>
     <row r="21" spans="1:14" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="B21" s="2">
         <v>25.4</v>
@@ -1981,10 +1959,10 @@
     </row>
     <row r="22" spans="1:14" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C22" s="1">
         <v>7</v>
@@ -2025,7 +2003,7 @@
     </row>
     <row r="23" spans="1:14" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="B23" s="2">
         <v>10.9</v>
@@ -2069,7 +2047,7 @@
     </row>
     <row r="24" spans="1:14" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="B24" s="2">
         <v>1540.9</v>
@@ -2113,7 +2091,7 @@
     </row>
     <row r="25" spans="1:14" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="B25" s="2">
         <v>21.9</v>
@@ -2157,7 +2135,7 @@
     </row>
     <row r="26" spans="1:14" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="B26" s="2">
         <v>81.099999999999994</v>
@@ -2201,7 +2179,7 @@
     </row>
     <row r="27" spans="1:14" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="B27" s="2">
         <v>7.4</v>
@@ -2245,7 +2223,7 @@
     </row>
     <row r="28" spans="1:14" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="B28" s="2">
         <v>5.6</v>
@@ -2289,7 +2267,7 @@
     </row>
     <row r="29" spans="1:14" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="B29" s="2">
         <v>0.6</v>
@@ -2333,10 +2311,10 @@
     </row>
     <row r="30" spans="1:14" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C30" s="2">
         <v>11.7</v>
@@ -2377,7 +2355,7 @@
     </row>
     <row r="31" spans="1:14" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="B31" s="2">
         <v>35.4</v>
@@ -2421,7 +2399,7 @@
     </row>
     <row r="32" spans="1:14" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="B32" s="2">
         <v>869.1</v>
@@ -2465,7 +2443,7 @@
     </row>
     <row r="33" spans="1:14" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="B33" s="2">
         <v>2.8</v>
@@ -2509,7 +2487,7 @@
     </row>
     <row r="34" spans="1:14" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="B34" s="2">
         <v>6.6</v>
@@ -2553,7 +2531,7 @@
     </row>
     <row r="35" spans="1:14" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="B35" s="2">
         <v>119.1</v>
@@ -2597,7 +2575,7 @@
     </row>
     <row r="36" spans="1:14" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="B36" s="2">
         <v>1727.7</v>
@@ -2641,7 +2619,7 @@
     </row>
     <row r="37" spans="1:14" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="B37" s="2">
         <v>255.8</v>
@@ -2685,7 +2663,7 @@
     </row>
     <row r="38" spans="1:14" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="B38" s="2">
         <v>1.1000000000000001</v>
@@ -2729,7 +2707,7 @@
     </row>
     <row r="39" spans="1:14" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="B39" s="2">
         <v>12.5</v>
@@ -2773,7 +2751,7 @@
     </row>
     <row r="40" spans="1:14" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="B40" s="1">
         <v>48</v>
@@ -2817,7 +2795,7 @@
     </row>
     <row r="41" spans="1:14" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="B41" s="2">
         <v>24.2</v>
@@ -2861,10 +2839,10 @@
     </row>
     <row r="42" spans="1:14" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="B42" s="1" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C42" s="2">
         <v>58.9</v>
@@ -2905,7 +2883,7 @@
     </row>
     <row r="43" spans="1:14" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="B43" s="1">
         <v>13</v>
@@ -2949,7 +2927,7 @@
     </row>
     <row r="44" spans="1:14" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="B44" s="2">
         <v>206.9</v>
@@ -2993,7 +2971,7 @@
     </row>
     <row r="45" spans="1:14" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="B45" s="2">
         <v>39.200000000000003</v>
@@ -3037,7 +3015,7 @@
     </row>
     <row r="46" spans="1:14" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="B46" s="2">
         <v>173.7</v>
@@ -3081,51 +3059,51 @@
     </row>
     <row r="47" spans="1:14" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="B47" s="1" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C47" s="2" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D47" s="2" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E47" s="2" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F47" s="2" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="G47" s="2">
         <v>2.2999999999999998</v>
       </c>
       <c r="H47" s="2" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="I47" s="2" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="J47" s="2" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="K47" s="2" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="L47" s="2" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="M47" s="2" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="N47" s="2" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="48" spans="1:14" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="B48" s="2">
         <v>0.5</v>
@@ -3169,7 +3147,7 @@
     </row>
     <row r="49" spans="1:14" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="B49" s="2">
         <v>39.299999999999997</v>
@@ -3213,7 +3191,7 @@
     </row>
     <row r="50" spans="1:14" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="B50" s="2">
         <v>76.3</v>
@@ -3257,7 +3235,7 @@
     </row>
     <row r="51" spans="1:14" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="B51" s="2">
         <v>331.1</v>
@@ -3301,7 +3279,7 @@
     </row>
     <row r="52" spans="1:14" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="B52" s="2">
         <v>23.8</v>
@@ -3345,7 +3323,7 @@
     </row>
     <row r="53" spans="1:14" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="B53" s="2">
         <v>0.4</v>
@@ -3389,10 +3367,10 @@
     </row>
     <row r="54" spans="1:14" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="B54" s="1" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C54" s="2">
         <v>4.9000000000000004</v>
@@ -3410,33 +3388,33 @@
         <v>6.8</v>
       </c>
       <c r="H54" s="2" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="I54" s="2" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="J54" s="2" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="K54" s="2" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="L54" s="2" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="M54" s="2" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="N54" s="2" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="55" spans="1:14" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="B55" s="1" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C55" s="2">
         <v>16.3</v>
@@ -3477,7 +3455,7 @@
     </row>
     <row r="56" spans="1:14" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="B56" s="2">
         <v>4.5999999999999996</v>
@@ -3521,7 +3499,7 @@
     </row>
     <row r="57" spans="1:14" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A57" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="B57" s="2">
         <v>31.4</v>
@@ -3565,7 +3543,7 @@
     </row>
     <row r="58" spans="1:14" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A58" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="B58" s="2">
         <v>4.3</v>
@@ -3609,7 +3587,7 @@
     </row>
     <row r="59" spans="1:14" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A59" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="B59" s="2">
         <v>144.1</v>
@@ -3653,7 +3631,7 @@
     </row>
     <row r="60" spans="1:14" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A60" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="B60" s="2">
         <v>1715.9</v>
@@ -3697,7 +3675,7 @@
     </row>
     <row r="61" spans="1:14" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A61" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="B61" s="2">
         <v>18.600000000000001</v>
@@ -3741,7 +3719,7 @@
     </row>
     <row r="62" spans="1:14" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A62" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="B62" s="2">
         <v>1.4</v>
@@ -3785,7 +3763,7 @@
     </row>
     <row r="63" spans="1:14" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A63" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="B63" s="2">
         <v>38.299999999999997</v>
@@ -3829,7 +3807,7 @@
     </row>
     <row r="64" spans="1:14" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A64" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="B64" s="2">
         <v>2485.1999999999998</v>
@@ -3871,9 +3849,9 @@
         <v>3811.3</v>
       </c>
     </row>
-    <row r="65" spans="1:15" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:14" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A65" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="B65" s="2">
         <v>28.1</v>
@@ -3915,9 +3893,9 @@
         <v>125.4</v>
       </c>
     </row>
-    <row r="66" spans="1:15" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="66" spans="1:14" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A66" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="B66" s="2">
         <v>210.9</v>
@@ -3959,9 +3937,9 @@
         <v>269.7</v>
       </c>
     </row>
-    <row r="67" spans="1:15" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="67" spans="1:14" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A67" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="B67" s="2">
         <v>0.7</v>
@@ -4003,9 +3981,9 @@
         <v>1.6</v>
       </c>
     </row>
-    <row r="68" spans="1:15" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="68" spans="1:14" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A68" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="B68" s="2">
         <v>47.3</v>
@@ -4047,9 +4025,9 @@
         <v>129.5</v>
       </c>
     </row>
-    <row r="69" spans="1:15" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="69" spans="1:14" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A69" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="B69" s="2">
         <v>8.5</v>
@@ -4091,9 +4069,9 @@
         <v>29</v>
       </c>
     </row>
-    <row r="70" spans="1:15" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="70" spans="1:14" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A70" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="B70" s="2">
         <v>1.6</v>
@@ -4135,9 +4113,9 @@
         <v>3</v>
       </c>
     </row>
-    <row r="71" spans="1:15" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="71" spans="1:14" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A71" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="B71" s="2">
         <v>2.1</v>
@@ -4179,9 +4157,9 @@
         <v>5.9</v>
       </c>
     </row>
-    <row r="72" spans="1:15" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="72" spans="1:14" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A72" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="B72" s="2">
         <v>14.9</v>
@@ -4223,9 +4201,9 @@
         <v>18.399999999999999</v>
       </c>
     </row>
-    <row r="73" spans="1:15" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="73" spans="1:14" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A73" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="B73" s="2">
         <v>15.9</v>
@@ -4267,9 +4245,9 @@
         <v>43.7</v>
       </c>
     </row>
-    <row r="74" spans="1:15" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="74" spans="1:14" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A74" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="B74" s="2">
         <v>153.9</v>
@@ -4311,12 +4289,12 @@
         <v>427.1</v>
       </c>
     </row>
-    <row r="75" spans="1:15" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="75" spans="1:14" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A75" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="B75" s="1" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C75" s="2">
         <v>158.30000000000001</v>
@@ -4355,9 +4333,9 @@
         <v>275.89999999999998</v>
       </c>
     </row>
-    <row r="76" spans="1:15" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="76" spans="1:14" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A76" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="B76" s="2">
         <v>7.7</v>
@@ -4399,9 +4377,9 @@
         <v>17.2</v>
       </c>
     </row>
-    <row r="77" spans="1:15" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="77" spans="1:14" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A77" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="B77" s="2">
         <v>1664.2</v>
@@ -4443,9 +4421,9 @@
         <v>9332</v>
       </c>
     </row>
-    <row r="78" spans="1:15" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="78" spans="1:14" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A78" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="B78" s="2">
         <v>839.2</v>
@@ -4487,9 +4465,9 @@
         <v>3106.5</v>
       </c>
     </row>
-    <row r="79" spans="1:15" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="79" spans="1:14" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A79" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="B79" s="2">
         <v>640.6</v>
@@ -4530,13 +4508,10 @@
       <c r="N79" s="2">
         <v>1540.7</v>
       </c>
-      <c r="O79" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="80" spans="1:15" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="80" spans="1:14" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A80" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="B80" s="2">
         <v>201.3</v>
@@ -4580,7 +4555,7 @@
     </row>
     <row r="81" spans="1:14" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A81" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="B81" s="2">
         <v>76.099999999999994</v>
@@ -4624,7 +4599,7 @@
     </row>
     <row r="82" spans="1:14" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A82" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="B82" s="2">
         <v>96.6</v>
@@ -4668,7 +4643,7 @@
     </row>
     <row r="83" spans="1:14" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A83" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="B83" s="2">
         <v>1766.3</v>
@@ -4712,7 +4687,7 @@
     </row>
     <row r="84" spans="1:14" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A84" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="B84" s="2">
         <v>17.7</v>
@@ -4756,7 +4731,7 @@
     </row>
     <row r="85" spans="1:14" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A85" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="B85" s="2">
         <v>3778.1</v>
@@ -4800,7 +4775,7 @@
     </row>
     <row r="86" spans="1:14" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A86" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="B86" s="2">
         <v>22.4</v>
@@ -4844,7 +4819,7 @@
     </row>
     <row r="87" spans="1:14" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A87" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="B87" s="2">
         <v>213.3</v>
@@ -4888,7 +4863,7 @@
     </row>
     <row r="88" spans="1:14" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A88" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="B88" s="2">
         <v>55.7</v>
@@ -4932,7 +4907,7 @@
     </row>
     <row r="89" spans="1:14" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A89" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="B89" s="2">
         <v>0.1</v>
@@ -4976,7 +4951,7 @@
     </row>
     <row r="90" spans="1:14" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A90" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="B90" s="2">
         <v>498.7</v>
@@ -5020,10 +4995,10 @@
     </row>
     <row r="91" spans="1:14" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A91" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="B91" s="1" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C91" s="2">
         <v>130.5</v>
@@ -5064,7 +5039,7 @@
     </row>
     <row r="92" spans="1:14" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A92" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="B92" s="2">
         <v>15.3</v>
@@ -5108,7 +5083,7 @@
     </row>
     <row r="93" spans="1:14" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A93" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="B93" s="2">
         <v>7.3</v>
@@ -5152,10 +5127,10 @@
     </row>
     <row r="94" spans="1:14" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A94" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="B94" s="1" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C94" s="2">
         <v>20.6</v>
@@ -5196,7 +5171,7 @@
     </row>
     <row r="95" spans="1:14" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A95" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="B95" s="2">
         <v>15.7</v>
@@ -5240,7 +5215,7 @@
     </row>
     <row r="96" spans="1:14" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A96" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="B96" s="2">
         <v>2.2000000000000002</v>
@@ -5284,13 +5259,13 @@
     </row>
     <row r="97" spans="1:14" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A97" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="B97" s="1" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C97" s="2" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D97" s="2">
         <v>3.8</v>
@@ -5328,13 +5303,13 @@
     </row>
     <row r="98" spans="1:14" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A98" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="B98" s="1" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C98" s="2" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D98" s="2">
         <v>117.4</v>
@@ -5372,10 +5347,10 @@
     </row>
     <row r="99" spans="1:14" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A99" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="B99" s="1" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C99" s="1">
         <v>34</v>
@@ -5416,7 +5391,7 @@
     </row>
     <row r="100" spans="1:14" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A100" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="B100" s="1">
         <v>22</v>
@@ -5460,7 +5435,7 @@
     </row>
     <row r="101" spans="1:14" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A101" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="B101" s="2">
         <v>19.2</v>
@@ -5504,7 +5479,7 @@
     </row>
     <row r="102" spans="1:14" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A102" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="B102" s="1">
         <v>7</v>
@@ -5548,7 +5523,7 @@
     </row>
     <row r="103" spans="1:14" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A103" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="B103" s="2">
         <v>190.3</v>
@@ -5592,10 +5567,10 @@
     </row>
     <row r="104" spans="1:14" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A104" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="B104" s="1" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C104" s="1">
         <v>2</v>
@@ -5636,7 +5611,7 @@
     </row>
     <row r="105" spans="1:14" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A105" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="B105" s="2">
         <v>10.8</v>
@@ -5680,7 +5655,7 @@
     </row>
     <row r="106" spans="1:14" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A106" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="B106" s="2">
         <v>5.7</v>
@@ -5724,7 +5699,7 @@
     </row>
     <row r="107" spans="1:14" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A107" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="B107" s="2">
         <v>0.1</v>
@@ -5768,7 +5743,7 @@
     </row>
     <row r="108" spans="1:14" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A108" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="B108" s="2">
         <v>5.7</v>
@@ -5812,7 +5787,7 @@
     </row>
     <row r="109" spans="1:14" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A109" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="B109" s="1">
         <v>8</v>
@@ -5856,7 +5831,7 @@
     </row>
     <row r="110" spans="1:14" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A110" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="B110" s="2">
         <v>1139.9000000000001</v>
@@ -5900,7 +5875,7 @@
     </row>
     <row r="111" spans="1:14" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A111" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="B111" s="2">
         <v>0.3</v>
@@ -5944,10 +5919,10 @@
     </row>
     <row r="112" spans="1:14" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A112" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="B112" s="1" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C112" s="2">
         <v>11.6</v>
@@ -5988,7 +5963,7 @@
     </row>
     <row r="113" spans="1:14" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A113" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="B113" s="2">
         <v>11.2</v>
@@ -6032,13 +6007,13 @@
     </row>
     <row r="114" spans="1:14" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A114" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="B114" s="1" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C114" s="2" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D114" s="2">
         <v>6.3</v>
@@ -6076,7 +6051,7 @@
     </row>
     <row r="115" spans="1:14" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A115" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="B115" s="2">
         <v>98.2</v>
@@ -6120,7 +6095,7 @@
     </row>
     <row r="116" spans="1:14" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A116" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="B116" s="1">
         <v>5</v>
@@ -6164,7 +6139,7 @@
     </row>
     <row r="117" spans="1:14" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A117" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="B117" s="2">
         <v>30.2</v>
@@ -6208,7 +6183,7 @@
     </row>
     <row r="118" spans="1:14" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A118" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="B118" s="2">
         <v>8.1999999999999993</v>
@@ -6252,19 +6227,19 @@
     </row>
     <row r="119" spans="1:14" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A119" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="B119" s="1" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C119" s="2" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D119" s="2" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E119" s="2" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F119" s="2">
         <v>0.1</v>
@@ -6296,7 +6271,7 @@
     </row>
     <row r="120" spans="1:14" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A120" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="B120" s="2">
         <v>22.5</v>
@@ -6340,7 +6315,7 @@
     </row>
     <row r="121" spans="1:14" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A121" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="B121" s="1">
         <v>483</v>
@@ -6384,7 +6359,7 @@
     </row>
     <row r="122" spans="1:14" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A122" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="B122" s="1">
         <v>80</v>
@@ -6428,7 +6403,7 @@
     </row>
     <row r="123" spans="1:14" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A123" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="B123" s="2">
         <v>12.4</v>
@@ -6472,7 +6447,7 @@
     </row>
     <row r="124" spans="1:14" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A124" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="B124" s="2">
         <v>7.2</v>
@@ -6516,7 +6491,7 @@
     </row>
     <row r="125" spans="1:14" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A125" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="B125" s="1">
         <v>320</v>
@@ -6560,7 +6535,7 @@
     </row>
     <row r="126" spans="1:14" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A126" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="B126" s="2">
         <v>19.2</v>
@@ -6604,7 +6579,7 @@
     </row>
     <row r="127" spans="1:14" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A127" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="B127" s="2">
         <v>181.6</v>
@@ -6648,7 +6623,7 @@
     </row>
     <row r="128" spans="1:14" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A128" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="B128" s="2">
         <v>63.5</v>
@@ -6692,7 +6667,7 @@
     </row>
     <row r="129" spans="1:14" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A129" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="B129" s="1">
         <v>329</v>
@@ -6736,13 +6711,13 @@
     </row>
     <row r="130" spans="1:14" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A130" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="B130" s="1" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C130" s="2" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D130" s="2">
         <v>0.2</v>
@@ -6780,10 +6755,10 @@
     </row>
     <row r="131" spans="1:14" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A131" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="B131" s="1" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C131" s="2">
         <v>8.1999999999999993</v>
@@ -6824,7 +6799,7 @@
     </row>
     <row r="132" spans="1:14" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A132" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="B132" s="2">
         <v>19.399999999999999</v>
@@ -6868,7 +6843,7 @@
     </row>
     <row r="133" spans="1:14" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A133" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="B133" s="2">
         <v>10.199999999999999</v>
@@ -6912,7 +6887,7 @@
     </row>
     <row r="134" spans="1:14" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A134" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="B134" s="2">
         <v>33.5</v>
@@ -6956,7 +6931,7 @@
     </row>
     <row r="135" spans="1:14" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A135" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="B135" s="1">
         <v>116</v>
@@ -7000,7 +6975,7 @@
     </row>
     <row r="136" spans="1:14" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A136" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="B136" s="2">
         <v>248.4</v>
@@ -7044,7 +7019,7 @@
     </row>
     <row r="137" spans="1:14" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A137" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="B137" s="2">
         <v>391.6</v>
@@ -7088,7 +7063,7 @@
     </row>
     <row r="138" spans="1:14" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A138" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="B138" s="2">
         <v>201.3</v>
@@ -7132,13 +7107,13 @@
     </row>
     <row r="139" spans="1:14" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A139" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="B139" s="1" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C139" s="2" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D139" s="2">
         <v>64.2</v>
@@ -7176,7 +7151,7 @@
     </row>
     <row r="140" spans="1:14" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A140" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="B140" s="2">
         <v>265.60000000000002</v>
@@ -7220,7 +7195,7 @@
     </row>
     <row r="141" spans="1:14" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A141" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="B141" s="2">
         <v>3094.5</v>
@@ -7264,7 +7239,7 @@
     </row>
     <row r="142" spans="1:14" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A142" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="B142" s="2">
         <v>6.3</v>
@@ -7308,7 +7283,7 @@
     </row>
     <row r="143" spans="1:14" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A143" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="B143" s="2">
         <v>0.6</v>
@@ -7352,7 +7327,7 @@
     </row>
     <row r="144" spans="1:14" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A144" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="B144" s="2">
         <v>1.3</v>
@@ -7394,9 +7369,9 @@
         <v>2.2000000000000002</v>
       </c>
     </row>
-    <row r="145" spans="1:15" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="145" spans="1:14" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A145" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="B145" s="2">
         <v>0.6</v>
@@ -7438,9 +7413,9 @@
         <v>1.2</v>
       </c>
     </row>
-    <row r="146" spans="1:15" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="146" spans="1:14" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A146" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="B146" s="2">
         <v>0.6</v>
@@ -7482,15 +7457,15 @@
         <v>1.2</v>
       </c>
     </row>
-    <row r="147" spans="1:15" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="147" spans="1:14" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A147" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="B147" s="1" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C147" s="2" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D147" s="2">
         <v>2.1</v>
@@ -7525,22 +7500,19 @@
       <c r="N147" s="2">
         <v>1.9</v>
       </c>
-      <c r="O147" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="148" spans="1:15" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="148" spans="1:14" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A148" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="B148" s="1" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C148" s="2" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D148" s="2" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E148" s="2">
         <v>0.3</v>
@@ -7573,9 +7545,9 @@
         <v>0.6</v>
       </c>
     </row>
-    <row r="149" spans="1:15" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="149" spans="1:14" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A149" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="B149" s="2">
         <v>693.2</v>
@@ -7617,9 +7589,9 @@
         <v>1651.1</v>
       </c>
     </row>
-    <row r="150" spans="1:15" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="150" spans="1:14" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A150" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="B150" s="2">
         <v>17.5</v>
@@ -7661,12 +7633,12 @@
         <v>53.2</v>
       </c>
     </row>
-    <row r="151" spans="1:15" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="151" spans="1:14" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A151" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="B151" s="1" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C151" s="1">
         <v>56</v>
@@ -7705,9 +7677,9 @@
         <v>112</v>
       </c>
     </row>
-    <row r="152" spans="1:15" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="152" spans="1:14" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A152" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="B152" s="1">
         <v>1</v>
@@ -7749,9 +7721,9 @@
         <v>2.6</v>
       </c>
     </row>
-    <row r="153" spans="1:15" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="153" spans="1:14" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A153" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="B153" s="2">
         <v>5.4</v>
@@ -7793,9 +7765,9 @@
         <v>10.9</v>
       </c>
     </row>
-    <row r="154" spans="1:15" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="154" spans="1:14" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A154" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="B154" s="2">
         <v>106.4</v>
@@ -7837,12 +7809,12 @@
         <v>508</v>
       </c>
     </row>
-    <row r="155" spans="1:15" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="155" spans="1:14" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A155" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="B155" s="1" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C155" s="2">
         <v>70.7</v>
@@ -7881,9 +7853,9 @@
         <v>170.6</v>
       </c>
     </row>
-    <row r="156" spans="1:15" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="156" spans="1:14" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A156" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="B156" s="2">
         <v>37.799999999999997</v>
@@ -7925,9 +7897,9 @@
         <v>67.7</v>
       </c>
     </row>
-    <row r="157" spans="1:15" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="157" spans="1:14" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A157" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="B157" s="2">
         <v>0.6</v>
@@ -7969,9 +7941,9 @@
         <v>1.4</v>
       </c>
     </row>
-    <row r="158" spans="1:15" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="158" spans="1:14" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A158" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="B158" s="2">
         <v>364.3</v>
@@ -8013,21 +7985,21 @@
         <v>701.6</v>
       </c>
     </row>
-    <row r="159" spans="1:15" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="159" spans="1:14" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A159" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="B159" s="1" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C159" s="2" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D159" s="2" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E159" s="2" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F159" s="2">
         <v>38.200000000000003</v>
@@ -8056,13 +8028,10 @@
       <c r="N159" s="2">
         <v>18.2</v>
       </c>
-      <c r="O159" t="s">
-        <v>162</v>
-      </c>
-    </row>
-    <row r="160" spans="1:15" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="160" spans="1:14" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A160" t="s">
-        <v>163</v>
+        <v>160</v>
       </c>
       <c r="B160" s="2">
         <v>923.4</v>
@@ -8106,7 +8075,7 @@
     </row>
     <row r="161" spans="1:14" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A161" t="s">
-        <v>164</v>
+        <v>161</v>
       </c>
       <c r="B161" s="2">
         <v>62.6</v>
@@ -8150,7 +8119,7 @@
     </row>
     <row r="162" spans="1:14" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A162" t="s">
-        <v>165</v>
+        <v>162</v>
       </c>
       <c r="B162" s="2">
         <v>45.2</v>
@@ -8194,7 +8163,7 @@
     </row>
     <row r="163" spans="1:14" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A163" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
       <c r="B163" s="2">
         <v>4.2</v>
@@ -8238,7 +8207,7 @@
     </row>
     <row r="164" spans="1:14" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A164" t="s">
-        <v>167</v>
+        <v>164</v>
       </c>
       <c r="B164" s="2">
         <v>265.10000000000002</v>
@@ -8282,7 +8251,7 @@
     </row>
     <row r="165" spans="1:14" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A165" t="s">
-        <v>168</v>
+        <v>165</v>
       </c>
       <c r="B165" s="2">
         <v>323.60000000000002</v>
@@ -8326,7 +8295,7 @@
     </row>
     <row r="166" spans="1:14" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A166" t="s">
-        <v>169</v>
+        <v>166</v>
       </c>
       <c r="B166" s="2">
         <v>19.3</v>
@@ -8370,7 +8339,7 @@
     </row>
     <row r="167" spans="1:14" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A167" t="s">
-        <v>170</v>
+        <v>167</v>
       </c>
       <c r="B167" s="2">
         <v>37.9</v>
@@ -8414,7 +8383,7 @@
     </row>
     <row r="168" spans="1:14" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A168" t="s">
-        <v>171</v>
+        <v>168</v>
       </c>
       <c r="B168" s="2">
         <v>376.3</v>
@@ -8458,13 +8427,13 @@
     </row>
     <row r="169" spans="1:14" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A169" t="s">
-        <v>172</v>
+        <v>169</v>
       </c>
       <c r="B169" s="1" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C169" s="2" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D169" s="2">
         <v>2.9</v>
@@ -8502,7 +8471,7 @@
     </row>
     <row r="170" spans="1:14" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A170" t="s">
-        <v>173</v>
+        <v>170</v>
       </c>
       <c r="B170" s="2">
         <v>4.9000000000000004</v>
@@ -8546,7 +8515,7 @@
     </row>
     <row r="171" spans="1:14" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A171" t="s">
-        <v>174</v>
+        <v>171</v>
       </c>
       <c r="B171" s="2">
         <v>0.3</v>
@@ -8590,7 +8559,7 @@
     </row>
     <row r="172" spans="1:14" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A172" t="s">
-        <v>175</v>
+        <v>172</v>
       </c>
       <c r="B172" s="2">
         <v>13.3</v>
@@ -8634,7 +8603,7 @@
     </row>
     <row r="173" spans="1:14" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A173" t="s">
-        <v>176</v>
+        <v>173</v>
       </c>
       <c r="B173" s="2">
         <v>46.2</v>
@@ -8678,7 +8647,7 @@
     </row>
     <row r="174" spans="1:14" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A174" t="s">
-        <v>177</v>
+        <v>174</v>
       </c>
       <c r="B174" s="2">
         <v>614.70000000000005</v>
@@ -8722,7 +8691,7 @@
     </row>
     <row r="175" spans="1:14" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A175" t="s">
-        <v>178</v>
+        <v>175</v>
       </c>
       <c r="B175" s="2">
         <v>30.6</v>
@@ -8766,7 +8735,7 @@
     </row>
     <row r="176" spans="1:14" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A176" t="s">
-        <v>179</v>
+        <v>176</v>
       </c>
       <c r="B176" s="1">
         <v>0</v>
@@ -8808,9 +8777,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="177" spans="1:15" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="177" spans="1:14" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A177" t="s">
-        <v>180</v>
+        <v>177</v>
       </c>
       <c r="B177" s="2">
         <v>13.4</v>
@@ -8852,9 +8821,9 @@
         <v>77.2</v>
       </c>
     </row>
-    <row r="178" spans="1:15" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="178" spans="1:14" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A178" t="s">
-        <v>181</v>
+        <v>178</v>
       </c>
       <c r="B178" s="1">
         <v>543</v>
@@ -8896,9 +8865,9 @@
         <v>346.9</v>
       </c>
     </row>
-    <row r="179" spans="1:15" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="179" spans="1:14" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A179" t="s">
-        <v>182</v>
+        <v>179</v>
       </c>
       <c r="B179" s="2">
         <v>205.4</v>
@@ -8940,9 +8909,9 @@
         <v>641.6</v>
       </c>
     </row>
-    <row r="180" spans="1:15" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="180" spans="1:14" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A180" t="s">
-        <v>183</v>
+        <v>180</v>
       </c>
       <c r="B180" s="2">
         <v>1527.1</v>
@@ -8984,9 +8953,9 @@
         <v>2670.1</v>
       </c>
     </row>
-    <row r="181" spans="1:15" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="181" spans="1:14" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A181" t="s">
-        <v>184</v>
+        <v>181</v>
       </c>
       <c r="B181" s="2">
         <v>9189.2999999999993</v>
@@ -9028,9 +8997,9 @@
         <v>18217</v>
       </c>
     </row>
-    <row r="182" spans="1:15" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="182" spans="1:14" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A182" t="s">
-        <v>185</v>
+        <v>182</v>
       </c>
       <c r="B182" s="2">
         <v>30.6</v>
@@ -9072,9 +9041,9 @@
         <v>72.099999999999994</v>
       </c>
     </row>
-    <row r="183" spans="1:15" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="183" spans="1:14" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A183" t="s">
-        <v>186</v>
+        <v>183</v>
       </c>
       <c r="B183" s="2">
         <v>63.4</v>
@@ -9116,9 +9085,9 @@
         <v>205.7</v>
       </c>
     </row>
-    <row r="184" spans="1:15" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="184" spans="1:14" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A184" t="s">
-        <v>187</v>
+        <v>184</v>
       </c>
       <c r="B184" s="2">
         <v>0.4</v>
@@ -9160,9 +9129,9 @@
         <v>0.8</v>
       </c>
     </row>
-    <row r="185" spans="1:15" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="185" spans="1:14" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A185" t="s">
-        <v>188</v>
+        <v>185</v>
       </c>
       <c r="B185" s="1">
         <v>287</v>
@@ -9203,13 +9172,10 @@
       <c r="N185" s="2">
         <v>514.70000000000005</v>
       </c>
-      <c r="O185" t="s">
-        <v>189</v>
-      </c>
-    </row>
-    <row r="186" spans="1:15" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="186" spans="1:14" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A186" t="s">
-        <v>190</v>
+        <v>186</v>
       </c>
       <c r="B186" s="2">
         <v>99.1</v>
@@ -9251,9 +9217,9 @@
         <v>631.4</v>
       </c>
     </row>
-    <row r="187" spans="1:15" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="187" spans="1:14" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A187" t="s">
-        <v>191</v>
+        <v>187</v>
       </c>
       <c r="B187" s="2">
         <v>40.1</v>
@@ -9295,9 +9261,9 @@
         <v>65.099999999999994</v>
       </c>
     </row>
-    <row r="188" spans="1:15" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="188" spans="1:14" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A188" t="s">
-        <v>192</v>
+        <v>188</v>
       </c>
       <c r="B188" s="2">
         <v>18.8</v>
@@ -9339,9 +9305,9 @@
         <v>65</v>
       </c>
     </row>
-    <row r="189" spans="1:15" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="189" spans="1:14" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A189" t="s">
-        <v>193</v>
+        <v>189</v>
       </c>
       <c r="B189" s="2">
         <v>29.4</v>
@@ -9383,180 +9349,180 @@
         <v>38.799999999999997</v>
       </c>
     </row>
-    <row r="190" spans="1:15" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="190" spans="1:14" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A190" t="s">
-        <v>194</v>
+        <v>190</v>
       </c>
       <c r="B190" s="1" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C190" s="2" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D190" s="2" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E190" s="2" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F190" s="2" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="G190" s="2" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="H190" s="2" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="I190" s="2" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="J190" s="2" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="K190" s="2" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="L190" s="2" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="M190" s="2" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="N190" s="2" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="191" spans="1:15" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="191" spans="1:14" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A191" t="s">
-        <v>195</v>
+        <v>191</v>
       </c>
       <c r="B191" s="1" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C191" s="2" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D191" s="2" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E191" s="2" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F191" s="2" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="G191" s="2" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="H191" s="2" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="I191" s="2" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="J191" s="2" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="K191" s="2" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="L191" s="2" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="M191" s="2" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="N191" s="2" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="192" spans="1:15" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="192" spans="1:14" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A192" t="s">
-        <v>196</v>
+        <v>192</v>
       </c>
       <c r="B192" s="1" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C192" s="2" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D192" s="2" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E192" s="2" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F192" s="2" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="G192" s="2" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="H192" s="2" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="I192" s="2" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="J192" s="2" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="K192" s="2" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="L192" s="2" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="M192" s="2" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="N192" s="2" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="193" spans="1:14" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A193" t="s">
-        <v>197</v>
+        <v>193</v>
       </c>
       <c r="B193" s="1" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C193" s="2" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D193" s="2" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E193" s="2" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F193" s="2" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="G193" s="2" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="H193" s="2" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="I193" s="2" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="J193" s="2" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="K193" s="2" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="L193" s="2" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="M193" s="2" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="N193" s="2" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="194" spans="1:14" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">

</xml_diff>